<commit_message>
Anova and Chi.Square Tests on the data for rebuttal
</commit_message>
<xml_diff>
--- a/Docs/Observational Study.xlsx
+++ b/Docs/Observational Study.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Development" sheetId="1" r:id="rId1"/>
     <sheet name="System Evaluation" sheetId="3" r:id="rId2"/>
+    <sheet name="Anova Test" sheetId="4" r:id="rId3"/>
+    <sheet name="Anova Test Results" sheetId="5" r:id="rId4"/>
+    <sheet name="Anova Test Results - Clean Data" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'System Evaluation'!$A$1:$K$65</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="65">
   <si>
     <t>Black</t>
   </si>
@@ -153,6 +159,63 @@
   </si>
   <si>
     <t>Count Stop</t>
+  </si>
+  <si>
+    <t>Anova: Single Factor</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Source of Variation</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>F crit</t>
+  </si>
+  <si>
+    <t>Between Groups</t>
+  </si>
+  <si>
+    <t>Within Groups</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Outliers have been removed</t>
   </si>
 </sst>
 </file>
@@ -163,7 +226,7 @@
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +235,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -195,12 +266,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -208,6 +299,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -997,11 +1093,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K49" sqref="A2:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1447,7 @@
         <v>1.9405925870850216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +1484,7 @@
         <v>1.9323733525072706</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1424,7 +1521,7 @@
         <v>1.9273715614594933</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1558,7 @@
         <v>1.932458674750154</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1498,7 +1595,7 @@
         <v>1.9348480601791995</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1535,7 +1632,7 @@
         <v>1.8773512546111981</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1669,7 @@
         <v>1.901484969214053</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1706,7 @@
         <v>1.9240170953650113</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1646,7 +1743,7 @@
         <v>1.9301004151379773</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1780,7 @@
         <v>1.9200113358602853</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1720,7 +1817,7 @@
         <v>1.9077410802583867</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1757,7 +1854,7 @@
         <v>1.9006734282577706</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1794,7 +1891,7 @@
         <v>1.9206914489216118</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1831,7 +1928,7 @@
         <v>1.9049619007619847</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1965,7 @@
         <v>1.9189939572105179</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1905,7 +2002,7 @@
         <v>1.9387087732411472</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1942,7 +2039,7 @@
         <v>1.9361865193013594</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1979,7 +2076,7 @@
         <v>1.926645174355915</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2113,7 @@
         <v>1.9306855892508379</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -2053,7 +2150,7 @@
         <v>1.9123121338989817</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -2090,7 +2187,7 @@
         <v>1.9301040007495549</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2224,7 @@
         <v>1.9075863240734305</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2164,7 +2261,7 @@
         <v>1.9299591973193322</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2201,7 +2298,7 @@
         <v>1.9041956012373733</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2238,7 +2335,7 @@
         <v>1.9263332867284959</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2275,7 +2372,7 @@
         <v>1.9164491273452842</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2409,7 @@
         <v>1.9225105533558036</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2446,7 @@
         <v>1.9030584868538722</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2386,7 +2483,7 @@
         <v>1.896043071306784</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2422,7 +2519,7 @@
         <v>1.6572096255622675</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2458,7 +2555,7 @@
         <v>1.8352888375969738</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2495,7 +2592,7 @@
         <v>1.9358287224975079</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2828,7 +2925,7 @@
         <v>1.9158763345549363</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2865,7 +2962,7 @@
         <v>1.9312298255455724</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +2999,7 @@
         <v>1.9323585460115051</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -2939,7 +3036,7 @@
         <v>1.9310732624040015</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -2976,7 +3073,7 @@
         <v>1.9287097651935914</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -3013,7 +3110,7 @@
         <v>1.9067016228630858</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3050,7 +3147,7 @@
         <v>1.9317011090236953</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -3087,7 +3184,7 @@
         <v>1.8597602975616476</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +3221,7 @@
         <v>1.8716871923119269</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -3161,7 +3258,7 @@
         <v>1.9162846622078606</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -3198,7 +3295,7 @@
         <v>1.9156844275858558</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3234,7 +3331,7 @@
         <v>1.8427778640721861</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -3271,7 +3368,7 @@
         <v>1.8914855436462024</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3308,7 +3405,7 @@
         <v>1.9095534040784115</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3345,7 +3442,7 @@
         <v>1.9158835872639359</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3382,7 +3479,7 @@
         <v>1.9392422879931188</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -3456,10 +3553,674 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K65">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="NoMask"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:I65">
     <sortCondition ref="D2:D65"/>
     <sortCondition ref="B2:B65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.6891891891891893E-2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3.5211267605633804E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4.0650406504065045E-3</v>
+      </c>
+      <c r="C6">
+        <v>7.6335877862595417E-3</v>
+      </c>
+      <c r="D6">
+        <v>1.1278195488721804E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.2048192771084338E-2</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1.1278195488721804E-2</v>
+      </c>
+      <c r="D8">
+        <v>4.0650406504065045E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3.8461538461538464E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.2641509433962263E-2</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>9.9009900990099011E-3</v>
+      </c>
+      <c r="D10">
+        <v>4.807692307692308E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.8726591760299626E-2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1.0067114093959731E-2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1.1406844106463879E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.2048192771084338E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1.1320754716981131E-2</v>
+      </c>
+      <c r="D13">
+        <v>7.9365079365079361E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7.9365079365079361E-3</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.2735042735042739E-3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1.2048192771084338E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1.2605042016806723E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.14450166914163051</v>
+      </c>
+      <c r="D5" s="7">
+        <v>9.031354321351907E-3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2.6079827056848685E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3.8070834962573318E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2.3794271851608323E-3</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2.0760736608718931E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.15329012850736035</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9.5806330317100216E-3</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4.6436445309751479E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>7.8822811215687835E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.9264257009804897E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.4156683292469762E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="7">
+        <v>5.6562597466627146E-4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.8854199155542381E-4</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.97933698527560198</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.40858026063378738</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2.7580782958425822</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1.1551202153507859E-2</v>
+      </c>
+      <c r="C14" s="7">
+        <v>60</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1.9252003589179765E-4</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.2116828128174131E-2</v>
+      </c>
+      <c r="C16" s="8">
+        <v>63</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7">
+        <v>8.2518198067250331E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5.5012132044833552E-3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>6.5794210380419886E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3.8070834962573318E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2.3794271851608323E-3</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2.0760736608718931E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3.1305395682932877E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2.2360996916380624E-3</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.5489499161818491E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8">
+        <v>7.8822811215687835E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.9264257009804897E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.4156683292469762E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1.3022344649294272E-4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4.3407815497647573E-5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.3774553185530507</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.25888658900313982</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2.7664379256680744</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1.796243732947349E-3</v>
+      </c>
+      <c r="C14" s="7">
+        <v>57</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3.1513047946444722E-5</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.9264671794402917E-3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>60</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>